<commit_message>
adding Ocean Resource Management Plan (ORMP) data layers as resilience layers to the OHI framework
</commit_message>
<xml_diff>
--- a/prep/HAB/hab_fishpond_numbers.xlsx
+++ b/prep/HAB/hab_fishpond_numbers.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/mhi/prep/HAB/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20115" windowHeight="10035"/>
+    <workbookView xWindow="12860" yWindow="1240" windowWidth="20120" windowHeight="10040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,6 +76,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -119,7 +127,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,9 +160,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,6 +212,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -362,16 +404,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -393,7 +435,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -406,7 +448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -417,7 +459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -434,24 +476,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>